<commit_message>
tests : constants : xlsx : WIP
</commit_message>
<xml_diff>
--- a/tests/data.gui/stable/emf/dsp.1/csv.comma/kev.emf.constants.data.xlsx
+++ b/tests/data.gui/stable/emf/dsp.1/csv.comma/kev.emf.constants.data.xlsx
@@ -270,10 +270,10 @@
     <t xml:space="preserve">OK</t>
   </si>
   <si>
-    <t xml:space="preserve">4.971923828125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0185485041910094</t>
+    <t xml:space="preserve">4.97236251831055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0185475079135167</t>
   </si>
   <si>
     <t xml:space="preserve">Adj. R^2</t>
@@ -709,7 +709,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.981564101396708</v>
+        <v>0.981565247999872</v>
       </c>
     </row>
   </sheetData>
@@ -1094,202 +1094,202 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.000320650751794945</v>
+        <v>0.000320489792950694</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00032745462855956</v>
+        <v>0.000327293669620107</v>
       </c>
       <c r="C2" t="n">
-        <v>2.80095503833757e-16</v>
+        <v>2.80236175548005e-16</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00984254080982287</v>
+        <v>0.00984270176871473</v>
       </c>
       <c r="E2" t="n">
-        <v>4.56161755220153e-09</v>
+        <v>4.56166515283288e-09</v>
       </c>
       <c r="F2" t="n">
-        <v>6.81300017301869e-06</v>
+        <v>6.81300017301839e-06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.000144934951673179</v>
+        <v>0.000144815394409726</v>
       </c>
       <c r="B3" t="n">
-        <v>0.000694492143695651</v>
+        <v>0.000694372558467839</v>
       </c>
       <c r="C3" t="n">
-        <v>4.99889027881563e-14</v>
+        <v>5.00301728233769e-14</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00943548645234059</v>
+        <v>0.00943560602358625</v>
       </c>
       <c r="E3" t="n">
-        <v>2.14039637703211e-08</v>
+        <v>2.14179459284501e-08</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000549600013251644</v>
+        <v>0.000549600013252206</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7.48952076072689e-05</v>
+        <v>7.48244161542317e-05</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00125674529994241</v>
+        <v>0.00125667437512966</v>
       </c>
       <c r="C4" t="n">
-        <v>2.08047957926759e-13</v>
+        <v>2.08244792301985e-13</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0088231797463292</v>
+        <v>0.0088232506044622</v>
       </c>
       <c r="E4" t="n">
-        <v>7.49537284068671e-08</v>
+        <v>7.50204081632837e-08</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00118200002666069</v>
+        <v>0.00118200002665783</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.47041594707056e-05</v>
+        <v>4.46602910627902e-05</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00193231800480312</v>
+        <v>0.00193227376593692</v>
       </c>
       <c r="C5" t="n">
-        <v>5.56742102803982e-13</v>
+        <v>5.57288973169373e-13</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00809748891814147</v>
+        <v>0.00809753297177881</v>
       </c>
       <c r="E5" t="n">
-        <v>1.930770554201e-07</v>
+        <v>1.93262284290596e-07</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00188800003973887</v>
+        <v>0.00188800003974056</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.29753781391267e-05</v>
+        <v>3.29426799300425e-05</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00244131397769643</v>
+        <v>0.00244128063203818</v>
       </c>
       <c r="C6" t="n">
-        <v>9.6304598320478e-13</v>
+        <v>9.64001882330223e-13</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00754635532256376</v>
+        <v>0.00754638834449791</v>
       </c>
       <c r="E6" t="n">
-        <v>3.3069973982554e-07</v>
+        <v>3.31023463932851e-07</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00240900004776922</v>
+        <v>0.0024090000477706</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.49047778656104e-05</v>
+        <v>2.48799403495712e-05</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00298283479417156</v>
+        <v>0.00298280889779496</v>
       </c>
       <c r="C7" t="n">
-        <v>1.56625438830958e-12</v>
+        <v>1.56781797198746e-12</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00696363021476453</v>
+        <v>0.00696365558171164</v>
       </c>
       <c r="E7" t="n">
-        <v>5.34991063900732e-07</v>
+        <v>5.35520493396148e-07</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00295900005522472</v>
+        <v>0.0029590000552358</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.25627165721912e-05</v>
+        <v>1.2550110653497e-05</v>
       </c>
       <c r="B8" t="n">
-        <v>0.00451335314998711</v>
+        <v>0.00451333733148972</v>
       </c>
       <c r="C8" t="n">
-        <v>4.72622971950048e-12</v>
+        <v>4.73097696589186e-12</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00531504206908348</v>
+        <v>0.00531505628129388</v>
       </c>
       <c r="E8" t="n">
-        <v>1.60478092942479e-06</v>
+        <v>1.60638721640046e-06</v>
       </c>
       <c r="F8" t="n">
-        <v>0.004504000069529</v>
+        <v>0.00450400006952423</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9.69699446366105e-06</v>
+        <v>9.68725679601052e-06</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00512397635747019</v>
+        <v>0.00512396188794407</v>
       </c>
       <c r="C9" t="n">
-        <v>6.9590184520488e-12</v>
+        <v>6.96601368405146e-12</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00465766332751259</v>
+        <v>0.00465767543111297</v>
       </c>
       <c r="E9" t="n">
-        <v>2.36031501722367e-06</v>
+        <v>2.36268094296218e-06</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00511900007246917</v>
+        <v>0.00511900007246139</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7.90192933202366e-06</v>
+        <v>7.8939927477496e-06</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0055975734801322</v>
+        <v>0.00559755919711815</v>
       </c>
       <c r="C10" t="n">
-        <v>9.33565018823056e-12</v>
+        <v>9.34503620840023e-12</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00414626229993571</v>
+        <v>0.00414627340973957</v>
       </c>
       <c r="E10" t="n">
-        <v>3.16421993208853e-06</v>
+        <v>3.16739314228429e-06</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00559600007329945</v>
+        <v>0.00559600007335086</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6.23532677520115e-06</v>
+        <v>6.22906538852753e-06</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00612346191648993</v>
+        <v>0.00612344685776672</v>
       </c>
       <c r="C11" t="n">
-        <v>1.29514316852232e-11</v>
+        <v>1.29644503190764e-11</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00357915138484314</v>
+        <v>0.00357916204490461</v>
       </c>
       <c r="E11" t="n">
-        <v>4.38669866691808e-06</v>
+        <v>4.39109732867863e-06</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0061260000728307</v>
+        <v>0.0061260000728142</v>
       </c>
     </row>
   </sheetData>
@@ -1352,34 +1352,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>162.849442866838</v>
+        <v>162.835364916109</v>
       </c>
       <c r="D2" t="n">
-        <v>140.585337275537</v>
+        <v>140.562199060342</v>
       </c>
       <c r="E2" t="n">
-        <v>122.074752109899</v>
+        <v>122.048237822434</v>
       </c>
       <c r="F2" t="n">
-        <v>107.606462597853</v>
+        <v>107.578935213466</v>
       </c>
       <c r="G2" t="n">
-        <v>99.0743324834217</v>
+        <v>99.0465163073831</v>
       </c>
       <c r="H2" t="n">
-        <v>91.2040093341404</v>
+        <v>91.1760330537543</v>
       </c>
       <c r="I2" t="n">
-        <v>72.0168347467973</v>
+        <v>71.9886861494901</v>
       </c>
       <c r="J2" t="n">
-        <v>64.7572942527332</v>
+        <v>64.7291244515028</v>
       </c>
       <c r="K2" t="n">
-        <v>59.0176516094977</v>
+        <v>58.9894764414753</v>
       </c>
       <c r="L2" t="n">
-        <v>52.3761111471282</v>
+        <v>52.3479417673376</v>
       </c>
     </row>
     <row r="3">
@@ -1390,34 +1390,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.850557133161942</v>
+        <v>-0.864635083891471</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.41466272446311</v>
+        <v>-1.4378009396579</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.22524789010117</v>
+        <v>-1.25176217756572</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.09353740214674</v>
+        <v>-3.12106478653401</v>
       </c>
       <c r="G3" t="n">
-        <v>-3.32566751657833</v>
+        <v>-3.35348369261688</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.99599066585958</v>
+        <v>-3.02396694624572</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.183165253202702</v>
+        <v>-0.211313850509924</v>
       </c>
       <c r="J3" t="n">
-        <v>1.2572942527332</v>
+        <v>1.22912445150278</v>
       </c>
       <c r="K3" t="n">
-        <v>3.01765160949771</v>
+        <v>2.98947644147531</v>
       </c>
       <c r="L3" t="n">
-        <v>8.1761111471282</v>
+        <v>8.14794176733763</v>
       </c>
     </row>
   </sheetData>
@@ -1480,34 +1480,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>162.849442866838</v>
+        <v>162.835364916109</v>
       </c>
       <c r="D2" t="n">
-        <v>140.585337275537</v>
+        <v>140.562199060342</v>
       </c>
       <c r="E2" t="n">
-        <v>122.074752109899</v>
+        <v>122.048237822434</v>
       </c>
       <c r="F2" t="n">
-        <v>107.606462597853</v>
+        <v>107.578935213466</v>
       </c>
       <c r="G2" t="n">
-        <v>99.0743324834217</v>
+        <v>99.0465163073831</v>
       </c>
       <c r="H2" t="n">
-        <v>91.2040093341404</v>
+        <v>91.1760330537543</v>
       </c>
       <c r="I2" t="n">
-        <v>72.0168347467973</v>
+        <v>71.9886861494901</v>
       </c>
       <c r="J2" t="n">
-        <v>64.7572942527332</v>
+        <v>64.7291244515028</v>
       </c>
       <c r="K2" t="n">
-        <v>59.0176516094977</v>
+        <v>58.9894764414753</v>
       </c>
       <c r="L2" t="n">
-        <v>52.3761111471282</v>
+        <v>52.3479417673376</v>
       </c>
     </row>
     <row r="3">
@@ -1518,34 +1518,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.00519582854711022</v>
+        <v>-0.00528182702438284</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.00996241355255714</v>
+        <v>-0.0101253587299852</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.00993712806245882</v>
+        <v>-0.010152166890233</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0279452339850654</v>
+        <v>-0.0281939005106956</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0324772218415853</v>
+        <v>-0.0327488641857117</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0318045718244117</v>
+        <v>-0.0321015599389142</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.00253691486430335</v>
+        <v>-0.00292678463310145</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0197999094918615</v>
+        <v>0.019356290574847</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0538866358838877</v>
+        <v>0.0533835078834877</v>
       </c>
       <c r="L3" t="n">
-        <v>0.18497989020652</v>
+        <v>0.184342573921666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>